<commit_message>
move to appropriate space
</commit_message>
<xml_diff>
--- a/data/excel/ship_capacity.xlsx
+++ b/data/excel/ship_capacity.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09C55DE-91CB-9242-A2BF-AC75E73D576A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5FC083-A209-E944-96D9-AD1A4B8D1AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="7240" windowWidth="28300" windowHeight="15900" xr2:uid="{A7C72FDA-F85C-FF4E-B260-3163B570FF28}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="15860" xr2:uid="{A7C72FDA-F85C-FF4E-B260-3163B570FF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>供給</t>
     <rPh sb="0" eb="2">
@@ -86,6 +86,16 @@
     </rPh>
     <rPh sb="7" eb="8">
       <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>三井住友銀行資料より</t>
+    <rPh sb="0" eb="6">
+      <t>ミツイスミテ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>シリョウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -451,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E659FFD5-7472-C140-94A0-4531B463AA71}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -463,99 +473,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>15000*1000000</f>
+        <v>15000000000</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <f>A3/B3</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <f>2000*1000000</f>
+        <v>2000000000</v>
+      </c>
+      <c r="B5">
+        <f>A5/12</f>
+        <v>166666666.66666666</v>
+      </c>
+      <c r="C5">
+        <f>B5/C3</f>
+        <v>55.55555555555555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
         <v>2000</v>
       </c>
-      <c r="B1">
+      <c r="B9">
         <v>1000000</v>
       </c>
-      <c r="C1">
+      <c r="C9">
         <v>9300</v>
       </c>
-      <c r="D1">
-        <f>A1*B1/C1</f>
+      <c r="D9">
+        <f>A9*B9/C9</f>
         <v>215053.7634408602</v>
       </c>
-      <c r="E1">
+      <c r="E9">
         <f>12</f>
         <v>12</v>
       </c>
-      <c r="F1">
-        <f>D1/E1</f>
+      <c r="F9">
+        <f>D9/E9</f>
         <v>17921.146953405016</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="10" spans="1:6">
+      <c r="A10">
         <v>15000</v>
       </c>
-      <c r="B2">
+      <c r="B10">
         <v>1000000</v>
       </c>
-      <c r="C2">
+      <c r="C10">
         <v>5000</v>
       </c>
-      <c r="D2">
-        <f>A2*B2/C2</f>
+      <c r="D10">
+        <f>A10*B10/C10</f>
         <v>3000000</v>
       </c>
-      <c r="F2">
-        <f>F1/D2</f>
+      <c r="F10">
+        <f>F9/D10</f>
         <v>5.9737156511350054E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="F3">
-        <f>F2*9300</f>
-        <v>55.55555555555555</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <f>15000*1000000</f>
-        <v>15000000000</v>
-      </c>
-      <c r="B6">
-        <v>5000</v>
-      </c>
-      <c r="C6">
-        <f>A6/B6</f>
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <f>2000*1000000</f>
-        <v>2000000000</v>
-      </c>
-      <c r="B8">
-        <f>A8/12</f>
-        <v>166666666.66666666</v>
-      </c>
-      <c r="C8">
-        <f>B8/C6</f>
+    <row r="11" spans="1:6">
+      <c r="F11">
+        <f>F10*9300</f>
         <v>55.55555555555555</v>
       </c>
     </row>

</xml_diff>